<commit_message>
Creating output to see how to put 4 day gaps between dates
</commit_message>
<xml_diff>
--- a/Fatigue_Data.xlsx
+++ b/Fatigue_Data.xlsx
@@ -452,47 +452,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>45972</v>
+        <v>45976</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>45973</v>
+        <v>45977</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>45974</v>
+        <v>45978</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>45975</v>
+        <v>45979</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
@@ -502,7 +502,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
@@ -512,7 +512,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -522,7 +522,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
@@ -532,841 +532,841 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45987</v>
+        <v>45970</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>45988</v>
+        <v>45971</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>45989</v>
+        <v>45972</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>45990</v>
+        <v>45973</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>45982</v>
+        <v>45988</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>45983</v>
+        <v>45989</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>45984</v>
+        <v>45990</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>45985</v>
+        <v>45991</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>45982</v>
+        <v>45993</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>45983</v>
+        <v>45994</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>45984</v>
+        <v>45995</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>45985</v>
+        <v>45996</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>45956</v>
+        <v>45997</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>45957</v>
+        <v>45998</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Ashlee Harper</t>
+          <t>Diane Paul</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>45958</v>
+        <v>45999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>45959</v>
+        <v>46000</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
-        <v>46001</v>
+        <v>45986</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>46002</v>
+        <v>45987</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>46003</v>
+        <v>45988</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>46004</v>
+        <v>45989</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>45950</v>
+        <v>46007</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>45951</v>
+        <v>46008</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>45952</v>
+        <v>46009</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>45953</v>
+        <v>46010</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
-        <v>45991</v>
+        <v>45959</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>45992</v>
+        <v>45960</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>45993</v>
+        <v>45961</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>45994</v>
+        <v>45962</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>45993</v>
+        <v>46012</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>45994</v>
+        <v>46013</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>45995</v>
+        <v>46014</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>45996</v>
+        <v>46015</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>45970</v>
+        <v>46019</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>45971</v>
+        <v>46020</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>45972</v>
+        <v>46021</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>45973</v>
+        <v>46022</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>45973</v>
+        <v>45983</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Eric Murphy</t>
+          <t>Kenneth Howell</t>
         </is>
       </c>
       <c r="B47" s="2" t="n">
-        <v>45974</v>
+        <v>45984</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>45975</v>
+        <v>45985</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B49" s="2" t="n">
-        <v>45976</v>
+        <v>45986</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B50" s="2" t="n">
-        <v>45945</v>
+        <v>45933</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B51" s="2" t="n">
-        <v>45946</v>
+        <v>45934</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B52" s="2" t="n">
-        <v>45947</v>
+        <v>45935</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B53" s="2" t="n">
-        <v>45948</v>
+        <v>45936</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B54" s="2" t="n">
-        <v>46015</v>
+        <v>46018</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B55" s="2" t="n">
-        <v>46016</v>
+        <v>46019</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B56" s="2" t="n">
-        <v>46017</v>
+        <v>46020</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B57" s="2" t="n">
-        <v>46018</v>
+        <v>46021</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B58" s="2" t="n">
-        <v>45942</v>
+        <v>45969</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B59" s="2" t="n">
-        <v>45943</v>
+        <v>45970</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B60" s="2" t="n">
-        <v>45944</v>
+        <v>45971</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B61" s="2" t="n">
-        <v>45945</v>
+        <v>45972</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B62" s="2" t="n">
-        <v>45955</v>
+        <v>45945</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B63" s="2" t="n">
-        <v>45956</v>
+        <v>45946</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B64" s="2" t="n">
-        <v>45957</v>
+        <v>45947</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B65" s="2" t="n">
-        <v>45958</v>
+        <v>45948</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B66" s="2" t="n">
-        <v>45982</v>
+        <v>45939</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B67" s="2" t="n">
-        <v>45983</v>
+        <v>45940</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B68" s="2" t="n">
-        <v>45984</v>
+        <v>45941</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B69" s="2" t="n">
-        <v>45985</v>
+        <v>45942</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>George Moore</t>
+          <t>Nancy Miller</t>
         </is>
       </c>
       <c r="B70" s="2" t="n">
-        <v>45961</v>
+        <v>45953</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B71" s="2" t="n">
-        <v>45962</v>
+        <v>45954</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B72" s="2" t="n">
-        <v>45963</v>
+        <v>45955</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B73" s="2" t="n">
-        <v>45964</v>
+        <v>45956</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B74" s="2" t="n">
-        <v>45986</v>
+        <v>46017</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B75" s="2" t="n">
-        <v>45987</v>
+        <v>46018</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B76" s="2" t="n">
-        <v>45988</v>
+        <v>46019</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B77" s="2" t="n">
-        <v>45989</v>
+        <v>46020</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B78" s="2" t="n">
-        <v>45931</v>
+        <v>46005</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B79" s="2" t="n">
-        <v>45932</v>
+        <v>46006</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B80" s="2" t="n">
-        <v>45933</v>
+        <v>46007</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B81" s="2" t="n">
-        <v>45934</v>
+        <v>46008</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B82" s="2" t="n">
-        <v>45995</v>
+        <v>46001</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B83" s="2" t="n">
-        <v>45996</v>
+        <v>46002</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B84" s="2" t="n">
-        <v>45997</v>
+        <v>46003</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B85" s="2" t="n">
-        <v>45998</v>
+        <v>46004</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B86" s="2" t="n">
-        <v>45939</v>
+        <v>45930</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B87" s="2" t="n">
-        <v>45940</v>
+        <v>45931</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B88" s="2" t="n">
-        <v>45941</v>
+        <v>45932</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B89" s="2" t="n">
-        <v>45942</v>
+        <v>45933</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B90" s="2" t="n">
-        <v>45963</v>
+        <v>45982</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B91" s="2" t="n">
-        <v>45964</v>
+        <v>45983</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B92" s="2" t="n">
-        <v>45965</v>
+        <v>45984</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Sarah Perez</t>
+          <t>Thomas Clarke</t>
         </is>
       </c>
       <c r="B93" s="2" t="n">
-        <v>45966</v>
+        <v>45985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>